<commit_message>
2nd Data Driven Test Case added
</commit_message>
<xml_diff>
--- a/MoneyControl_DDD/src/test/resources/testdata/testdata.xlsx
+++ b/MoneyControl_DDD/src/test/resources/testdata/testdata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Softwares\Automation\MoneyControl_DDD\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Softwares\SeleniumWorkspace\MoneyControl_DDD\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C492503C-A442-4C9D-B371-52B63A621684}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="calculateTax" sheetId="1" r:id="rId1"/>
+    <sheet name="calculateCarLoan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Taxable_Amount</t>
   </si>
@@ -40,12 +40,33 @@
   </si>
   <si>
     <t>VERY SENIOR CITIZEN</t>
+  </si>
+  <si>
+    <t>Loan_Amount</t>
+  </si>
+  <si>
+    <t>Loan_Period</t>
+  </si>
+  <si>
+    <t>EMI_Starts_From</t>
+  </si>
+  <si>
+    <t>Interest_Rate</t>
+  </si>
+  <si>
+    <t>Upfront_Charges</t>
+  </si>
+  <si>
+    <t>At the time of loan disbursement</t>
+  </si>
+  <si>
+    <t>From next month after disbursement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,20 +377,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -377,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1200000</v>
       </c>
@@ -385,7 +406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000000</v>
       </c>
@@ -393,12 +414,83 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>900000</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2000000</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>6.5</v>
+      </c>
+      <c r="E2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1500000</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>